<commit_message>
Added paq8l results on images
</commit_message>
<xml_diff>
--- a/Resuts/images.xlsx
+++ b/Resuts/images.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="23256" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="images" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t>Filename</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>woman_darkhair</t>
+  </si>
+  <si>
+    <t>PAQ8L -5</t>
   </si>
 </sst>
 </file>
@@ -662,247 +665,7 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1256,10 +1019,10 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
@@ -1310,6 +1073,9 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
       <c r="R1" t="s">
         <v>16</v>
       </c>
@@ -1372,6 +1138,9 @@
       <c r="P2">
         <v>146902</v>
       </c>
+      <c r="Q2">
+        <v>104844</v>
+      </c>
       <c r="R2">
         <v>91554</v>
       </c>
@@ -1379,6 +1148,7 @@
         <v>91530</v>
       </c>
       <c r="U2">
+        <f>MIN(C2:T2)</f>
         <v>91530</v>
       </c>
     </row>
@@ -1431,6 +1201,9 @@
       <c r="P3">
         <v>184160</v>
       </c>
+      <c r="Q3">
+        <v>111421</v>
+      </c>
       <c r="S3">
         <v>91548</v>
       </c>
@@ -1438,6 +1211,7 @@
         <v>161180</v>
       </c>
       <c r="U3">
+        <f t="shared" ref="U3:U51" si="0">MIN(C3:T3)</f>
         <v>91548</v>
       </c>
     </row>
@@ -1490,6 +1264,9 @@
       <c r="P5">
         <v>107792</v>
       </c>
+      <c r="Q5">
+        <v>74341</v>
+      </c>
       <c r="R5">
         <v>63116</v>
       </c>
@@ -1497,6 +1274,7 @@
         <v>63096</v>
       </c>
       <c r="U5">
+        <f t="shared" si="0"/>
         <v>63096</v>
       </c>
     </row>
@@ -1549,6 +1327,9 @@
       <c r="P6">
         <v>136837</v>
       </c>
+      <c r="Q6">
+        <v>81598</v>
+      </c>
       <c r="S6">
         <v>63114</v>
       </c>
@@ -1556,6 +1337,7 @@
         <v>116297</v>
       </c>
       <c r="U6">
+        <f t="shared" si="0"/>
         <v>63114</v>
       </c>
     </row>
@@ -1608,6 +1390,9 @@
       <c r="P8">
         <v>174863</v>
       </c>
+      <c r="Q8">
+        <v>133231</v>
+      </c>
       <c r="R8">
         <v>127933</v>
       </c>
@@ -1615,6 +1400,7 @@
         <v>127903</v>
       </c>
       <c r="U8">
+        <f t="shared" si="0"/>
         <v>127903</v>
       </c>
     </row>
@@ -1667,6 +1453,9 @@
       <c r="P9">
         <v>193675</v>
       </c>
+      <c r="Q9">
+        <v>137030</v>
+      </c>
       <c r="S9">
         <v>127921</v>
       </c>
@@ -1674,6 +1463,7 @@
         <v>190156</v>
       </c>
       <c r="U9">
+        <f t="shared" si="0"/>
         <v>127921</v>
       </c>
     </row>
@@ -1726,6 +1516,9 @@
       <c r="P11">
         <v>221014</v>
       </c>
+      <c r="Q11">
+        <v>165481</v>
+      </c>
       <c r="R11">
         <v>1654293</v>
       </c>
@@ -1733,6 +1526,7 @@
         <v>164271</v>
       </c>
       <c r="U11">
+        <f t="shared" si="0"/>
         <v>164271</v>
       </c>
     </row>
@@ -1785,6 +1579,9 @@
       <c r="P12">
         <v>232958</v>
       </c>
+      <c r="Q12">
+        <v>170451</v>
+      </c>
       <c r="S12">
         <v>164289</v>
       </c>
@@ -1792,6 +1589,7 @@
         <v>225842</v>
       </c>
       <c r="U12">
+        <f t="shared" si="0"/>
         <v>164289</v>
       </c>
     </row>
@@ -1844,6 +1642,9 @@
       <c r="P14">
         <v>203482</v>
       </c>
+      <c r="Q14">
+        <v>101749</v>
+      </c>
       <c r="R14">
         <v>105882</v>
       </c>
@@ -1851,7 +1652,8 @@
         <v>105861</v>
       </c>
       <c r="U14">
-        <v>105861</v>
+        <f t="shared" si="0"/>
+        <v>101749</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1903,6 +1705,9 @@
       <c r="P15">
         <v>202486</v>
       </c>
+      <c r="Q15">
+        <v>110141</v>
+      </c>
       <c r="S15">
         <v>105861</v>
       </c>
@@ -1910,6 +1715,7 @@
         <v>102917</v>
       </c>
       <c r="U15">
+        <f t="shared" si="0"/>
         <v>102917</v>
       </c>
     </row>
@@ -1962,6 +1768,9 @@
       <c r="P17">
         <v>761995</v>
       </c>
+      <c r="Q17">
+        <v>419751</v>
+      </c>
       <c r="R17">
         <v>445105</v>
       </c>
@@ -1969,7 +1778,8 @@
         <v>445074</v>
       </c>
       <c r="U17">
-        <v>445074</v>
+        <f t="shared" si="0"/>
+        <v>419751</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -2021,6 +1831,9 @@
       <c r="P18">
         <v>763062</v>
       </c>
+      <c r="Q18">
+        <v>434828</v>
+      </c>
       <c r="S18">
         <v>445074</v>
       </c>
@@ -2028,7 +1841,8 @@
         <v>443449</v>
       </c>
       <c r="U18">
-        <v>443449</v>
+        <f t="shared" si="0"/>
+        <v>434828</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2080,6 +1894,9 @@
       <c r="P20">
         <v>62193</v>
       </c>
+      <c r="Q20">
+        <v>42593</v>
+      </c>
       <c r="R20">
         <v>40610</v>
       </c>
@@ -2087,6 +1904,7 @@
         <v>40586</v>
       </c>
       <c r="U20">
+        <f t="shared" si="0"/>
         <v>40586</v>
       </c>
     </row>
@@ -2139,6 +1957,9 @@
       <c r="P21">
         <v>71766</v>
       </c>
+      <c r="Q21">
+        <v>44774</v>
+      </c>
       <c r="S21">
         <v>40604</v>
       </c>
@@ -2146,6 +1967,7 @@
         <v>56025</v>
       </c>
       <c r="U21">
+        <f t="shared" si="0"/>
         <v>40604</v>
       </c>
     </row>
@@ -2198,6 +2020,9 @@
       <c r="P23">
         <v>202624</v>
       </c>
+      <c r="Q23">
+        <v>150892</v>
+      </c>
       <c r="R23">
         <v>141074</v>
       </c>
@@ -2205,6 +2030,7 @@
         <v>141052</v>
       </c>
       <c r="U23">
+        <f t="shared" si="0"/>
         <v>141052</v>
       </c>
     </row>
@@ -2257,6 +2083,9 @@
       <c r="P24">
         <v>215872</v>
       </c>
+      <c r="Q24">
+        <v>157128</v>
+      </c>
       <c r="S24">
         <v>141070</v>
       </c>
@@ -2264,6 +2093,7 @@
         <v>205302</v>
       </c>
       <c r="U24">
+        <f t="shared" si="0"/>
         <v>141070</v>
       </c>
     </row>
@@ -2316,6 +2146,9 @@
       <c r="P26">
         <v>216184</v>
       </c>
+      <c r="Q26">
+        <v>161751</v>
+      </c>
       <c r="R26">
         <v>159626</v>
       </c>
@@ -2323,6 +2156,7 @@
         <v>159605</v>
       </c>
       <c r="U26">
+        <f t="shared" si="0"/>
         <v>159605</v>
       </c>
     </row>
@@ -2375,6 +2209,9 @@
       <c r="P27">
         <v>232381</v>
       </c>
+      <c r="Q27">
+        <v>167761</v>
+      </c>
       <c r="S27">
         <v>159623</v>
       </c>
@@ -2382,6 +2219,7 @@
         <v>220711</v>
       </c>
       <c r="U27">
+        <f t="shared" si="0"/>
         <v>159623</v>
       </c>
     </row>
@@ -2434,6 +2272,9 @@
       <c r="P29">
         <v>516373</v>
       </c>
+      <c r="Q29">
+        <v>418559</v>
+      </c>
       <c r="R29">
         <v>608774</v>
       </c>
@@ -2441,7 +2282,8 @@
         <v>608751</v>
       </c>
       <c r="U29">
-        <v>471286</v>
+        <f t="shared" si="0"/>
+        <v>418559</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -2493,6 +2335,9 @@
       <c r="P30">
         <v>514765</v>
       </c>
+      <c r="Q30">
+        <v>369978</v>
+      </c>
       <c r="S30">
         <v>608751</v>
       </c>
@@ -2500,7 +2345,8 @@
         <v>606161</v>
       </c>
       <c r="U30">
-        <v>472696</v>
+        <f t="shared" si="0"/>
+        <v>369978</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -2552,6 +2398,9 @@
       <c r="P32">
         <v>231089</v>
       </c>
+      <c r="Q32">
+        <v>168377</v>
+      </c>
       <c r="R32">
         <v>137670</v>
       </c>
@@ -2559,6 +2408,7 @@
         <v>137647</v>
       </c>
       <c r="U32">
+        <f t="shared" si="0"/>
         <v>137647</v>
       </c>
     </row>
@@ -2611,6 +2461,9 @@
       <c r="P33">
         <v>246711</v>
       </c>
+      <c r="Q33">
+        <v>175107</v>
+      </c>
       <c r="S33">
         <v>137665</v>
       </c>
@@ -2618,6 +2471,7 @@
         <v>231870</v>
       </c>
       <c r="U33">
+        <f t="shared" si="0"/>
         <v>137665</v>
       </c>
     </row>
@@ -2670,6 +2524,9 @@
       <c r="P35">
         <v>129227</v>
       </c>
+      <c r="Q35">
+        <v>93893</v>
+      </c>
       <c r="R35">
         <v>511977</v>
       </c>
@@ -2677,7 +2534,8 @@
         <v>511951</v>
       </c>
       <c r="U35">
-        <v>118674</v>
+        <f t="shared" si="0"/>
+        <v>93893</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -2729,6 +2587,9 @@
       <c r="P36">
         <v>138105</v>
       </c>
+      <c r="Q36">
+        <v>99407</v>
+      </c>
       <c r="S36">
         <v>511951</v>
       </c>
@@ -2736,7 +2597,8 @@
         <v>505875</v>
       </c>
       <c r="U36">
-        <v>136358</v>
+        <f t="shared" si="0"/>
+        <v>99407</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -2788,6 +2650,9 @@
       <c r="P38">
         <v>119864</v>
       </c>
+      <c r="Q38">
+        <v>90057</v>
+      </c>
       <c r="R38">
         <v>159348</v>
       </c>
@@ -2795,7 +2660,8 @@
         <v>159329</v>
       </c>
       <c r="U38">
-        <v>111754</v>
+        <f t="shared" si="0"/>
+        <v>90057</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -2847,6 +2713,9 @@
       <c r="P39">
         <v>152580</v>
       </c>
+      <c r="Q39">
+        <v>97288</v>
+      </c>
       <c r="S39">
         <v>159347</v>
       </c>
@@ -2854,7 +2723,8 @@
         <v>218665</v>
       </c>
       <c r="U39">
-        <v>135843</v>
+        <f t="shared" si="0"/>
+        <v>97288</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -2906,6 +2776,9 @@
       <c r="P41">
         <v>209697</v>
       </c>
+      <c r="Q41">
+        <v>161060</v>
+      </c>
       <c r="R41">
         <v>155338</v>
       </c>
@@ -2913,6 +2786,7 @@
         <v>155316</v>
       </c>
       <c r="U41">
+        <f t="shared" si="0"/>
         <v>155316</v>
       </c>
     </row>
@@ -2965,6 +2839,9 @@
       <c r="P42">
         <v>220749</v>
       </c>
+      <c r="Q42">
+        <v>165515</v>
+      </c>
       <c r="S42">
         <v>155334</v>
       </c>
@@ -2972,6 +2849,7 @@
         <v>215596</v>
       </c>
       <c r="U42">
+        <f t="shared" si="0"/>
         <v>155334</v>
       </c>
     </row>
@@ -3024,6 +2902,9 @@
       <c r="P44">
         <v>248820</v>
       </c>
+      <c r="Q44">
+        <v>186724</v>
+      </c>
       <c r="R44">
         <v>184069</v>
       </c>
@@ -3031,6 +2912,7 @@
         <v>184046</v>
       </c>
       <c r="U44">
+        <f t="shared" si="0"/>
         <v>184046</v>
       </c>
     </row>
@@ -3083,6 +2965,9 @@
       <c r="P45">
         <v>267027</v>
       </c>
+      <c r="Q45">
+        <v>191005</v>
+      </c>
       <c r="S45">
         <v>184064</v>
       </c>
@@ -3090,6 +2975,7 @@
         <v>246415</v>
       </c>
       <c r="U45">
+        <f t="shared" si="0"/>
         <v>184064</v>
       </c>
     </row>
@@ -3142,6 +3028,9 @@
       <c r="P47">
         <v>204320</v>
       </c>
+      <c r="Q47">
+        <v>151350</v>
+      </c>
       <c r="R47">
         <v>158642</v>
       </c>
@@ -3149,7 +3038,8 @@
         <v>158623</v>
       </c>
       <c r="U47">
-        <v>158623</v>
+        <f t="shared" si="0"/>
+        <v>151350</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -3201,6 +3091,9 @@
       <c r="P48">
         <v>215773</v>
       </c>
+      <c r="Q48">
+        <v>162092</v>
+      </c>
       <c r="S48">
         <v>158641</v>
       </c>
@@ -3208,6 +3101,7 @@
         <v>220817</v>
       </c>
       <c r="U48">
+        <f t="shared" si="0"/>
         <v>158641</v>
       </c>
     </row>
@@ -3260,6 +3154,9 @@
       <c r="P50">
         <v>157780</v>
       </c>
+      <c r="Q50">
+        <v>121024</v>
+      </c>
       <c r="R50">
         <v>111833</v>
       </c>
@@ -3267,6 +3164,7 @@
         <v>111804</v>
       </c>
       <c r="U50">
+        <f t="shared" si="0"/>
         <v>111804</v>
       </c>
     </row>
@@ -3319,6 +3217,9 @@
       <c r="P51">
         <v>173340</v>
       </c>
+      <c r="Q51">
+        <v>125600</v>
+      </c>
       <c r="S51">
         <v>111822</v>
       </c>
@@ -3326,21 +3227,22 @@
         <v>117961</v>
       </c>
       <c r="U51">
+        <f t="shared" si="0"/>
         <v>111822</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D37:U51 D31:U35 D19:U29 D2:U14 D16:U17">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+  <conditionalFormatting sqref="D37:U51 D31:U35 D19:U29 D2:U14 D16:U17 U3:U51">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:U36">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:U30">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:U18">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:U15">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>